<commit_message>
penbmi for template 1
penbmi for template 1
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="35">
   <si>
     <t>Benchmarks</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>PolySynth</t>
-  </si>
-  <si>
-    <t>invSDP</t>
   </si>
   <si>
     <t>ex1</t>
@@ -108,7 +105,7 @@
     </r>
   </si>
   <si>
-    <t>inv=a0+a1*x1+a2*x2
+    <t>a0+a1*x1+a2*x2
 a3*x1^2+a4*x2^2+a5*x1*x2</t>
   </si>
   <si>
@@ -127,16 +124,13 @@
     <t>Template 2</t>
   </si>
   <si>
-    <t>PresetN</t>
+    <t>invSDP</t>
   </si>
   <si>
     <t>1+a1*x1+a2*x1^2</t>
   </si>
   <si>
     <t>1+a1*x1^2+a2*x2^2</t>
-  </si>
-  <si>
-    <t>4次以下无解</t>
   </si>
   <si>
     <t>ex4</t>
@@ -1358,20 +1352,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="11.05" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="6" max="8" width="9.375"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" spans="1:7">
+    <row r="1" ht="14.25" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1390,16 +1384,13 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+    </row>
+    <row r="2" ht="14.25" spans="1:6">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" ht="14.25" spans="1:7">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="2">
         <v>0.29</v>
@@ -1408,40 +1399,38 @@
         <v>0.75</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" ht="28.5" spans="1:6">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" ht="28.5" spans="1:7">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="C3" s="2">
         <v>0.45</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" ht="14.25" spans="1:7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2">
         <v>0.29</v>
@@ -1450,19 +1439,18 @@
         <v>0.56</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" ht="14.25" spans="1:7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="2">
         <v>0.32</v>
@@ -1474,16 +1462,15 @@
         <v>0.63</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" ht="14.25" spans="1:7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" ht="14.25" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2">
         <v>0.32</v>
@@ -1497,387 +1484,330 @@
       <c r="F6" s="1">
         <v>0.514</v>
       </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" ht="28.5" spans="1:7">
+    </row>
+    <row r="7" ht="28.5" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2">
         <v>0.67</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" ht="28.5" spans="1:7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" ht="28.5" spans="1:6">
       <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="C8" s="2">
         <v>1.18</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" ht="28.5" spans="1:7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" ht="28.5" spans="1:6">
       <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1.33</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" ht="28.5" spans="1:6">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" ht="28.5" spans="1:7">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="B10" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2">
         <v>0.72</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" ht="28.5" spans="1:7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" ht="28.5" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2">
         <v>0.7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="3">
         <v>0.84</v>
       </c>
-      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="7:7">
       <c r="G12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25" spans="1:7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25" spans="1:6">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="1" t="s">
+    </row>
+    <row r="17" ht="14.25" spans="1:6">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" ht="14.25" spans="1:7">
-      <c r="A17" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1.86</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25" spans="1:6">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1.86</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="18" ht="14.25" spans="1:8">
-      <c r="A18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2">
+        <v>1.02</v>
+      </c>
+      <c r="D18" s="1">
+        <v>7.18</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" ht="14.25" spans="1:6">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.35</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="20" ht="14.25" spans="1:6">
+      <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="1">
-        <v>4</v>
-      </c>
-      <c r="D18" s="2">
-        <v>1.02</v>
-      </c>
-      <c r="E18" s="1">
-        <v>7.18</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" ht="14.25" spans="1:7">
-      <c r="A19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0.35</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="20" ht="14.25" spans="1:7">
-      <c r="A20" s="1" t="s">
+      <c r="C20" s="2">
+        <v>0.34</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.527</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" ht="14.25" spans="1:6">
+      <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1.1</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.535</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" ht="14.25" spans="1:6">
+      <c r="A22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.34</v>
-      </c>
-      <c r="E20" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0.527</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" ht="14.25" spans="1:7">
-      <c r="A21" s="1" t="s">
+      <c r="C22" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" ht="29" customHeight="1" spans="1:6">
+      <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.31</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1.1</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0.535</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" ht="14.25" spans="1:8">
-      <c r="A22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="1">
-        <v>3</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.39</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" ht="29" customHeight="1" spans="1:8">
-      <c r="A23" s="1" t="s">
+      <c r="C23" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" ht="14.25" spans="1:6">
+      <c r="A24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C24" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" ht="28" customHeight="1" spans="1:6">
+      <c r="A25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C23" s="2">
-        <v>2</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.87</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" ht="14.25" spans="1:8">
-      <c r="A24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="C25" s="2">
+        <v>19.06</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.866</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" ht="28" customHeight="1" spans="1:6">
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="2">
-        <v>2</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0.87</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0.21</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" ht="28" customHeight="1" spans="1:8">
-      <c r="A25" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="2">
-        <v>2</v>
-      </c>
-      <c r="D25" s="2">
-        <v>19.06</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0.866</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" ht="28" customHeight="1" spans="1:8">
-      <c r="A26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="C26" s="2">
-        <v>2</v>
-      </c>
-      <c r="D26" s="2">
         <v>1.62</v>
       </c>
+      <c r="D26" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="E26" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H26" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>